<commit_message>
Real expressions for an auto pdf excel filler
</commit_message>
<xml_diff>
--- a/biofire_pdf_data.xlsx
+++ b/biofire_pdf_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -548,7 +548,22 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Negative</t>
         </is>
       </c>
     </row>
@@ -575,7 +590,22 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Adenovirus CoronavirusOC43 SevereAcuteRespiratorySyndromeCoronavirus2(SARS-CoV-2)HumanMetapneumovirus HumanRhinovirus/Enterovirus InfluenzaAH1-2009 InfluenzaAH3 InfluenzaB ParainfluenzaVirus1 ParainfluenzaVirus2 ParainfluenzaVirus3 ParainfluenzaVirus4 RespiratorySyncytialVirus Bordetellaparapertussis(IS1001) Bordetellapertussis(ptxP) Chlamydiapneumoniae Mycoplasmapneumoniae</t>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Positive</t>
         </is>
       </c>
     </row>

</xml_diff>